<commit_message>
Dev V2 - Need to finish it quick - corner block detection done - working on compatibility of cell traceback with external operations (like unpivotr etc) - read_cells / complete huristic detection can also be made like Table_List - mark cell-analysis for remodeling into state (may be in laster version) - added test Article (FileTypes) - multi routes tests - introduce grammer - todo %<^% kind of symbols for NNE etc - No merge to stable before next version
</commit_message>
<xml_diff>
--- a/00_nightly_only/file_samples/blocks.xlsx
+++ b/00_nightly_only/file_samples/blocks.xlsx
@@ -7,8 +7,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Empty" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Empty" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="17">
   <si>
     <t>a</t>
   </si>
@@ -44,6 +45,33 @@
   </si>
   <si>
     <t>disconnected</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>leaf</t>
+  </si>
+  <si>
+    <t>leaf 2</t>
+  </si>
+  <si>
+    <t>OMG Leaf</t>
+  </si>
+  <si>
+    <t>leaf 3</t>
+  </si>
+  <si>
+    <t>leaf 1</t>
   </si>
 </sst>
 </file>
@@ -377,10 +405,181 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J17"/>
+  <dimension ref="C7:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="J22" sqref="J22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1">
+        <v>3</v>
+      </c>
+      <c r="H9" s="1">
+        <v>4</v>
+      </c>
+      <c r="I9" s="1">
+        <v>5</v>
+      </c>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>3</v>
+      </c>
+      <c r="H10" s="1">
+        <v>4</v>
+      </c>
+      <c r="I10" s="1">
+        <v>5</v>
+      </c>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1">
+        <v>3</v>
+      </c>
+      <c r="H11" s="1">
+        <v>4</v>
+      </c>
+      <c r="I11" s="1">
+        <v>5</v>
+      </c>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1">
+        <v>3</v>
+      </c>
+      <c r="H12" s="1">
+        <v>4</v>
+      </c>
+      <c r="I12" s="1">
+        <v>5</v>
+      </c>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>3</v>
+      </c>
+      <c r="H13" s="1">
+        <v>4</v>
+      </c>
+      <c r="I13" s="1">
+        <v>5</v>
+      </c>
+      <c r="J13" s="1"/>
+      <c r="L13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="D14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+      <c r="K15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="M16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:N33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21:N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,9 +646,184 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:14" x14ac:dyDescent="0.25">
       <c r="J17" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="L22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="E23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="E24" s="1"/>
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1">
+        <v>2</v>
+      </c>
+      <c r="H24" s="1">
+        <v>3</v>
+      </c>
+      <c r="I24" s="1">
+        <v>4</v>
+      </c>
+      <c r="J24" s="1">
+        <v>5</v>
+      </c>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="E25" s="1"/>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1">
+        <v>2</v>
+      </c>
+      <c r="H25" s="1">
+        <v>3</v>
+      </c>
+      <c r="I25" s="1">
+        <v>4</v>
+      </c>
+      <c r="J25" s="1">
+        <v>5</v>
+      </c>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="E26" s="1"/>
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
+      <c r="G26" s="1">
+        <v>2</v>
+      </c>
+      <c r="H26" s="1">
+        <v>3</v>
+      </c>
+      <c r="I26" s="1">
+        <v>4</v>
+      </c>
+      <c r="J26" s="1">
+        <v>5</v>
+      </c>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="E27" s="1"/>
+      <c r="F27" s="1">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1">
+        <v>2</v>
+      </c>
+      <c r="H27" s="1">
+        <v>3</v>
+      </c>
+      <c r="I27" s="1">
+        <v>4</v>
+      </c>
+      <c r="J27" s="1">
+        <v>5</v>
+      </c>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="E28" s="1"/>
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1">
+        <v>2</v>
+      </c>
+      <c r="H28" s="1">
+        <v>3</v>
+      </c>
+      <c r="I28" s="1">
+        <v>4</v>
+      </c>
+      <c r="J28" s="1">
+        <v>5</v>
+      </c>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="E29" s="1"/>
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
+      <c r="G29" s="1">
+        <v>2</v>
+      </c>
+      <c r="H29" s="1">
+        <v>3</v>
+      </c>
+      <c r="I29" s="1">
+        <v>4</v>
+      </c>
+      <c r="J29" s="1">
+        <v>5</v>
+      </c>
+      <c r="K29" s="1"/>
+      <c r="M29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="E30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>16</v>
+      </c>
+      <c r="L31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>13</v>
+      </c>
+      <c r="N32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -457,7 +831,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>